<commit_message>
Terminado todos os desenhos
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheron_carneiro\Documents\FORMULA1_NOVO\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzo_reis\Documents\Enzo\VFX\game_test\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -282,12 +282,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -302,12 +308,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +997,7 @@
       <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1011,7 +1018,7 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1048,7 +1055,7 @@
       <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1077,7 +1084,7 @@
       <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1098,7 +1105,7 @@
       <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feito desenha, função principal e variáveis
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1005,7 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>